<commit_message>
updating fullerene data spreadsheet
</commit_message>
<xml_diff>
--- a/sknano/data/fullerenes/Cn_fullerenes.xlsx
+++ b/sknano/data/fullerenes/Cn_fullerenes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="12" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="875" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="13" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="875" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="C20" sheetId="1" state="visible" r:id="rId2"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="25">
   <si>
     <t>#</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>S4</t>
+  </si>
+  <si>
+    <t>C2h</t>
   </si>
   <si>
     <t>None</t>
@@ -2300,8 +2303,8 @@
   </sheetPr>
   <dimension ref="A1:C117"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A70" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C118" activeCellId="0" pane="topLeft" sqref="C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2320,584 +2323,1280 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>30.405</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="3">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="B3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>27.337</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="4">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="B4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>28.111</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="5">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="B5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>27.805</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="6">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="B6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>27.129</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="7">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="B7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>28.221</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="8">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="B8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>27.585</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="9">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
+      <c r="B9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>26.77</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="10">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
+      <c r="B10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>28.473</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="11">
       <c r="A11" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>27.819</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="12">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
+      <c r="B12" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>27.401</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="13">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
+      <c r="B13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>26.825</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="14">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
+      <c r="B14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>25.99</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="15">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
+      <c r="B15" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>26.263</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="16">
       <c r="A16" s="0" t="n">
         <v>15</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>28.076</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="17">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="B17" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>26.843</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="18">
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
+      <c r="B18" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>26.501</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="19">
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
+      <c r="B19" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>26.377</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="20">
       <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
+      <c r="B20" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>26.621</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="21">
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="B21" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>28.709</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="22">
       <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
+      <c r="B22" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>27.152</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="23">
       <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
+      <c r="B23" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>26.061</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="24">
       <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
+      <c r="B24" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>25.562</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="25">
       <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
+      <c r="B25" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>25.631</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="26">
       <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
+      <c r="B26" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>25.64</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="27">
       <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
+      <c r="B27" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>26.607</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="28">
       <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
+      <c r="B28" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>26.224</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="29">
       <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
+      <c r="B29" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>25.888</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="30">
       <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
+      <c r="B30" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>25.451</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="31">
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="B31" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>25.247</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="32">
       <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
+      <c r="B32" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>27.241</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="33">
       <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="B33" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>25.439</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="34">
       <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
+      <c r="B34" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>27.644</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="35">
       <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
+      <c r="B35" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>25.632</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="36">
       <c r="A36" s="0" t="n">
         <v>35</v>
       </c>
+      <c r="B36" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>24.951</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="37">
       <c r="A37" s="0" t="n">
         <v>36</v>
       </c>
+      <c r="B37" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>24.757</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="38">
       <c r="A38" s="0" t="n">
         <v>37</v>
       </c>
+      <c r="B38" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>26.261</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="39">
       <c r="A39" s="0" t="n">
         <v>38</v>
       </c>
+      <c r="B39" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>25.907</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="40">
       <c r="A40" s="0" t="n">
         <v>39</v>
       </c>
+      <c r="B40" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>25.323</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="41">
       <c r="A41" s="0" t="n">
         <v>40</v>
       </c>
+      <c r="B41" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>24.492</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="42">
       <c r="A42" s="0" t="n">
         <v>41</v>
       </c>
+      <c r="B42" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>25.471</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="43">
       <c r="A43" s="0" t="n">
         <v>42</v>
       </c>
+      <c r="B43" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>27.582</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="44">
       <c r="A44" s="0" t="n">
         <v>43</v>
       </c>
+      <c r="B44" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>25.589</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="45">
       <c r="A45" s="0" t="n">
         <v>44</v>
       </c>
+      <c r="B45" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>25.351</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="46">
       <c r="A46" s="0" t="n">
         <v>45</v>
       </c>
+      <c r="B46" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>26.618</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="47">
       <c r="A47" s="0" t="n">
         <v>46</v>
       </c>
+      <c r="B47" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>25.132</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="48">
       <c r="A48" s="0" t="n">
         <v>47</v>
       </c>
+      <c r="B48" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>26.054</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="49">
       <c r="A49" s="0" t="n">
         <v>48</v>
       </c>
+      <c r="B49" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>26.898</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="50">
       <c r="A50" s="0" t="n">
         <v>49</v>
       </c>
+      <c r="B50" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>26.299</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="51">
       <c r="A51" s="0" t="n">
         <v>50</v>
       </c>
+      <c r="B51" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>25.054</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="52">
       <c r="A52" s="0" t="n">
         <v>51</v>
       </c>
+      <c r="B52" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>25.219</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="53">
       <c r="A53" s="0" t="n">
         <v>52</v>
       </c>
+      <c r="B53" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>25.719</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="54">
       <c r="A54" s="0" t="n">
         <v>53</v>
       </c>
+      <c r="B54" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>26.177</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="55">
       <c r="A55" s="0" t="n">
         <v>54</v>
       </c>
+      <c r="B55" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>24.938</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="56">
       <c r="A56" s="0" t="n">
         <v>55</v>
       </c>
+      <c r="B56" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>24.869</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="57">
       <c r="A57" s="0" t="n">
         <v>56</v>
       </c>
+      <c r="B57" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>25.737</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="58">
       <c r="A58" s="0" t="n">
         <v>57</v>
       </c>
+      <c r="B58" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>26.421</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="59">
       <c r="A59" s="0" t="n">
         <v>58</v>
       </c>
+      <c r="B59" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>25.544</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="60">
       <c r="A60" s="0" t="n">
         <v>59</v>
       </c>
+      <c r="B60" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>25.024</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="61">
       <c r="A61" s="0" t="n">
         <v>60</v>
       </c>
+      <c r="B61" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>24.257</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="62">
       <c r="A62" s="0" t="n">
         <v>61</v>
       </c>
+      <c r="B62" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>24.272</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="63">
       <c r="A63" s="0" t="n">
         <v>62</v>
       </c>
+      <c r="B63" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C63" s="0" t="n">
+        <v>24.946</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="64">
       <c r="A64" s="0" t="n">
         <v>63</v>
       </c>
+      <c r="B64" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>24.378</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="65">
       <c r="A65" s="0" t="n">
         <v>64</v>
       </c>
+      <c r="B65" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>25.331</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="66">
       <c r="A66" s="0" t="n">
         <v>65</v>
       </c>
+      <c r="B66" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>24.613</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="67">
       <c r="A67" s="0" t="n">
         <v>66</v>
       </c>
+      <c r="B67" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C67" s="0" t="n">
+        <v>24.204</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="68">
       <c r="A68" s="0" t="n">
         <v>67</v>
       </c>
+      <c r="B68" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C68" s="0" t="n">
+        <v>23.851</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="69">
       <c r="A69" s="0" t="n">
         <v>68</v>
       </c>
+      <c r="B69" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C69" s="0" t="n">
+        <v>24.521</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="70">
       <c r="A70" s="0" t="n">
         <v>69</v>
       </c>
+      <c r="B70" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" s="0" t="n">
+        <v>24.186</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="71">
       <c r="A71" s="0" t="n">
         <v>70</v>
       </c>
+      <c r="B71" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" s="0" t="n">
+        <v>24.039</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="72">
       <c r="A72" s="0" t="n">
         <v>71</v>
       </c>
+      <c r="B72" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C72" s="0" t="n">
+        <v>24.983</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="73">
       <c r="A73" s="0" t="n">
         <v>72</v>
       </c>
+      <c r="B73" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C73" s="0" t="n">
+        <v>24.167</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="74">
       <c r="A74" s="0" t="n">
         <v>73</v>
       </c>
+      <c r="B74" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C74" s="0" t="n">
+        <v>24.637</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="75">
       <c r="A75" s="0" t="n">
         <v>74</v>
       </c>
+      <c r="B75" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C75" s="0" t="n">
+        <v>24.188</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="76">
       <c r="A76" s="0" t="n">
         <v>75</v>
       </c>
+      <c r="B76" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C76" s="0" t="n">
+        <v>24.612</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="77">
       <c r="A77" s="0" t="n">
         <v>76</v>
       </c>
+      <c r="B77" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <v>24.884</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="78">
       <c r="A78" s="0" t="n">
         <v>77</v>
       </c>
+      <c r="B78" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C78" s="0" t="n">
+        <v>25.388</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="79">
       <c r="A79" s="0" t="n">
         <v>78</v>
       </c>
+      <c r="B79" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>24.596</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="80">
       <c r="A80" s="0" t="n">
         <v>79</v>
       </c>
+      <c r="B80" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80" s="0" t="n">
+        <v>24.275</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="81">
       <c r="A81" s="0" t="n">
         <v>80</v>
       </c>
+      <c r="B81" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C81" s="0" t="n">
+        <v>24.963</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="82">
       <c r="A82" s="0" t="n">
         <v>81</v>
       </c>
+      <c r="B82" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C82" s="0" t="n">
+        <v>24.523</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="83">
       <c r="A83" s="0" t="n">
         <v>82</v>
       </c>
+      <c r="B83" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C83" s="0" t="n">
+        <v>24.558</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="84">
       <c r="A84" s="0" t="n">
         <v>83</v>
       </c>
+      <c r="B84" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C84" s="0" t="n">
+        <v>25.265</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="85">
       <c r="A85" s="0" t="n">
         <v>84</v>
       </c>
+      <c r="B85" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C85" s="0" t="n">
+        <v>24.33</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="86">
       <c r="A86" s="0" t="n">
         <v>85</v>
       </c>
+      <c r="B86" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C86" s="0" t="n">
+        <v>23.608</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="87">
       <c r="A87" s="0" t="n">
         <v>86</v>
       </c>
+      <c r="B87" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C87" s="0" t="n">
+        <v>23.325</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="88">
       <c r="A88" s="0" t="n">
         <v>87</v>
       </c>
+      <c r="B88" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C88" s="0" t="n">
+        <v>23.562</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="89">
       <c r="A89" s="0" t="n">
         <v>88</v>
       </c>
+      <c r="B89" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C89" s="0" t="n">
+        <v>23.282</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="90">
       <c r="A90" s="0" t="n">
         <v>89</v>
       </c>
+      <c r="B90" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C90" s="0" t="n">
+        <v>24.467</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="91">
       <c r="A91" s="0" t="n">
         <v>90</v>
       </c>
+      <c r="B91" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C91" s="0" t="n">
+        <v>23.253</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="92">
       <c r="A92" s="0" t="n">
         <v>91</v>
       </c>
+      <c r="B92" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C92" s="0" t="n">
+        <v>24.685</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="93">
       <c r="A93" s="0" t="n">
         <v>92</v>
       </c>
+      <c r="B93" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C93" s="0" t="n">
+        <v>23.934</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="94">
       <c r="A94" s="0" t="n">
         <v>93</v>
       </c>
+      <c r="B94" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C94" s="0" t="n">
+        <v>23.589</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="95">
       <c r="A95" s="0" t="n">
         <v>94</v>
       </c>
+      <c r="B95" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C95" s="0" t="n">
+        <v>23.011</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="96">
       <c r="A96" s="0" t="n">
         <v>95</v>
       </c>
+      <c r="B96" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C96" s="0" t="n">
+        <v>23.55</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="97">
       <c r="A97" s="0" t="n">
         <v>96</v>
       </c>
+      <c r="B97" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C97" s="0" t="n">
+        <v>24.017</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="98">
       <c r="A98" s="0" t="n">
         <v>97</v>
       </c>
+      <c r="B98" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C98" s="0" t="n">
+        <v>24.433</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="99">
       <c r="A99" s="0" t="n">
         <v>98</v>
       </c>
+      <c r="B99" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C99" s="0" t="n">
+        <v>23.813</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="100">
       <c r="A100" s="0" t="n">
         <v>99</v>
       </c>
+      <c r="B100" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C100" s="0" t="n">
+        <v>23.465</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="101">
       <c r="A101" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="B101" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C101" s="0" t="n">
+        <v>23.779</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="102">
       <c r="A102" s="0" t="n">
         <v>101</v>
       </c>
+      <c r="B102" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C102" s="0" t="n">
+        <v>23.419</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="103">
       <c r="A103" s="0" t="n">
         <v>102</v>
       </c>
+      <c r="B103" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C103" s="0" t="n">
+        <v>23.58</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="104">
       <c r="A104" s="0" t="n">
         <v>103</v>
       </c>
+      <c r="B104" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C104" s="0" t="n">
+        <v>23.069</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="105">
       <c r="A105" s="0" t="n">
         <v>104</v>
       </c>
+      <c r="B105" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C105" s="0" t="n">
+        <v>23.245</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="106">
       <c r="A106" s="0" t="n">
         <v>105</v>
       </c>
+      <c r="B106" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C106" s="0" t="n">
+        <v>23.855</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="107">
       <c r="A107" s="0" t="n">
         <v>106</v>
       </c>
+      <c r="B107" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C107" s="0" t="n">
+        <v>23.274</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="108">
       <c r="A108" s="0" t="n">
         <v>107</v>
       </c>
+      <c r="B108" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C108" s="0" t="n">
+        <v>23.273</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="109">
       <c r="A109" s="0" t="n">
         <v>108</v>
       </c>
+      <c r="B109" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C109" s="0" t="n">
+        <v>22.958</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="110">
       <c r="A110" s="0" t="n">
         <v>109</v>
       </c>
+      <c r="B110" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C110" s="0" t="n">
+        <v>22.769</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="111">
       <c r="A111" s="0" t="n">
         <v>110</v>
       </c>
+      <c r="B111" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C111" s="0" t="n">
+        <v>23.101</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="112">
       <c r="A112" s="0" t="n">
         <v>111</v>
       </c>
+      <c r="B112" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C112" s="0" t="n">
+        <v>23.674</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="113">
       <c r="A113" s="0" t="n">
         <v>112</v>
       </c>
+      <c r="B113" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C113" s="0" t="n">
+        <v>23.576</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="114">
       <c r="A114" s="0" t="n">
         <v>113</v>
       </c>
+      <c r="B114" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C114" s="0" t="n">
+        <v>25.297</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="115">
       <c r="A115" s="0" t="n">
         <v>114</v>
       </c>
+      <c r="B115" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C115" s="0" t="n">
+        <v>22.671</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="116">
       <c r="A116" s="0" t="n">
         <v>115</v>
       </c>
+      <c r="B116" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C116" s="0" t="n">
+        <v>23.093</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="117">
       <c r="A117" s="0" t="n">
         <v>116</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C117" s="0" t="n">
+        <v>22.705</v>
       </c>
     </row>
   </sheetData>
@@ -2918,8 +3617,8 @@
   </sheetPr>
   <dimension ref="A1:C200"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A89" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B122" activeCellId="0" pane="topLeft" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2942,600 +3641,1320 @@
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="B2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>30.885</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="3">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="B3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>36.058</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="4">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="B4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>28.913</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="5">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="B5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>28.725</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="6">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="B6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>31.082</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="7">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="B7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>29.523</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="8">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="B8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>28.404</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="9">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
+      <c r="B9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>27.765</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="10">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
+      <c r="B10" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>29.493</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="11">
       <c r="A11" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>27.401</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="12">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
+      <c r="B12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>27.834</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="13">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
+      <c r="B13" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>29.653</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="14">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
+      <c r="B14" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>28.115</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="15">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
+      <c r="B15" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>29.372</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="16">
       <c r="A16" s="0" t="n">
         <v>15</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>29.264</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="17">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="B17" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>28.861</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="18">
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
+      <c r="B18" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>27.597</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="19">
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
+      <c r="B19" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>27.262</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="20">
       <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
+      <c r="B20" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>26.626</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="21">
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="B21" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>27.66</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="22">
       <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
+      <c r="B22" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>27.155</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="23">
       <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
+      <c r="B23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>26.229</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="24">
       <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
+      <c r="B24" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>27.337</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="25">
       <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
+      <c r="B25" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>27.637</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="26">
       <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
+      <c r="B26" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>27.275</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="27">
       <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
+      <c r="B27" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>28.008</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="28">
       <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
+      <c r="B28" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>28.479</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="29">
       <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
+      <c r="B29" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>26.279</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="30">
       <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
+      <c r="B30" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>27.085</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="31">
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="B31" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>28.325</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="32">
       <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
+      <c r="B32" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>28.005</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="33">
       <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="B33" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>26.419</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="34">
       <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
+      <c r="B34" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>25.713</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="35">
       <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
+      <c r="B35" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>25.984</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="36">
       <c r="A36" s="0" t="n">
         <v>35</v>
       </c>
+      <c r="B36" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>27.251</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="37">
       <c r="A37" s="0" t="n">
         <v>36</v>
       </c>
+      <c r="B37" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>26.464</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="38">
       <c r="A38" s="0" t="n">
         <v>37</v>
       </c>
+      <c r="B38" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>26.189</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="39">
       <c r="A39" s="0" t="n">
         <v>38</v>
       </c>
+      <c r="B39" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>25.618</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="40">
       <c r="A40" s="0" t="n">
         <v>39</v>
       </c>
+      <c r="B40" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>25.491</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="41">
       <c r="A41" s="0" t="n">
         <v>40</v>
       </c>
+      <c r="B41" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>26.118</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="42">
       <c r="A42" s="0" t="n">
         <v>41</v>
       </c>
+      <c r="B42" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>26.017</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="43">
       <c r="A43" s="0" t="n">
         <v>42</v>
       </c>
+      <c r="B43" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>25.443</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="44">
       <c r="A44" s="0" t="n">
         <v>43</v>
       </c>
+      <c r="B44" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>26.179</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="45">
       <c r="A45" s="0" t="n">
         <v>44</v>
       </c>
+      <c r="B45" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>25.464</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="46">
       <c r="A46" s="0" t="n">
         <v>45</v>
       </c>
+      <c r="B46" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>25.72</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="47">
       <c r="A47" s="0" t="n">
         <v>46</v>
       </c>
+      <c r="B47" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>28.924</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="48">
       <c r="A48" s="0" t="n">
         <v>47</v>
       </c>
+      <c r="B48" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>25.515</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="49">
       <c r="A49" s="0" t="n">
         <v>48</v>
       </c>
+      <c r="B49" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>26.744</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="50">
       <c r="A50" s="0" t="n">
         <v>49</v>
       </c>
+      <c r="B50" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>29.797</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="51">
       <c r="A51" s="0" t="n">
         <v>50</v>
       </c>
+      <c r="B51" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>25.872</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="52">
       <c r="A52" s="0" t="n">
         <v>51</v>
       </c>
+      <c r="B52" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>25.167</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="53">
       <c r="A53" s="0" t="n">
         <v>52</v>
       </c>
+      <c r="B53" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>26.139</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="54">
       <c r="A54" s="0" t="n">
         <v>53</v>
       </c>
+      <c r="B54" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>25.501</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="55">
       <c r="A55" s="0" t="n">
         <v>54</v>
       </c>
+      <c r="B55" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>26.065</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="56">
       <c r="A56" s="0" t="n">
         <v>55</v>
       </c>
+      <c r="B56" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>25.991</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="57">
       <c r="A57" s="0" t="n">
         <v>56</v>
       </c>
+      <c r="B57" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>26.45</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="58">
       <c r="A58" s="0" t="n">
         <v>57</v>
       </c>
+      <c r="B58" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>27.946</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="59">
       <c r="A59" s="0" t="n">
         <v>58</v>
       </c>
+      <c r="B59" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>25.791</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="60">
       <c r="A60" s="0" t="n">
         <v>59</v>
       </c>
+      <c r="B60" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>28.118</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="61">
       <c r="A61" s="0" t="n">
         <v>60</v>
       </c>
+      <c r="B61" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>26.821</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="62">
       <c r="A62" s="0" t="n">
         <v>61</v>
       </c>
+      <c r="B62" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>25.325</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="63">
       <c r="A63" s="0" t="n">
         <v>62</v>
       </c>
+      <c r="B63" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63" s="0" t="n">
+        <v>25.195</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="64">
       <c r="A64" s="0" t="n">
         <v>63</v>
       </c>
+      <c r="B64" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>28.206</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="65">
       <c r="A65" s="0" t="n">
         <v>64</v>
       </c>
+      <c r="B65" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>26.554</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="66">
       <c r="A66" s="0" t="n">
         <v>65</v>
       </c>
+      <c r="B66" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>25.931</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="67">
       <c r="A67" s="0" t="n">
         <v>66</v>
       </c>
+      <c r="B67" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" s="0" t="n">
+        <v>26.278</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="68">
       <c r="A68" s="0" t="n">
         <v>67</v>
       </c>
+      <c r="B68" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C68" s="0" t="n">
+        <v>25.344</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="69">
       <c r="A69" s="0" t="n">
         <v>68</v>
       </c>
+      <c r="B69" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C69" s="0" t="n">
+        <v>26.913</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="70">
       <c r="A70" s="0" t="n">
         <v>69</v>
       </c>
+      <c r="B70" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" s="0" t="n">
+        <v>27.326</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="71">
       <c r="A71" s="0" t="n">
         <v>70</v>
       </c>
+      <c r="B71" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C71" s="0" t="n">
+        <v>27.083</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="72">
       <c r="A72" s="0" t="n">
         <v>71</v>
       </c>
+      <c r="B72" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C72" s="0" t="n">
+        <v>24.95</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="73">
       <c r="A73" s="0" t="n">
         <v>72</v>
       </c>
+      <c r="B73" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C73" s="0" t="n">
+        <v>25.032</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="74">
       <c r="A74" s="0" t="n">
         <v>73</v>
       </c>
+      <c r="B74" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C74" s="0" t="n">
+        <v>24.87</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="75">
       <c r="A75" s="0" t="n">
         <v>74</v>
       </c>
+      <c r="B75" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C75" s="0" t="n">
+        <v>25.326</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="76">
       <c r="A76" s="0" t="n">
         <v>75</v>
       </c>
+      <c r="B76" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C76" s="0" t="n">
+        <v>25.979</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="77">
       <c r="A77" s="0" t="n">
         <v>76</v>
       </c>
+      <c r="B77" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <v>26.552</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="78">
       <c r="A78" s="0" t="n">
         <v>77</v>
       </c>
+      <c r="B78" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C78" s="0" t="n">
+        <v>25.225</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="79">
       <c r="A79" s="0" t="n">
         <v>78</v>
       </c>
+      <c r="B79" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>25.439</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="80">
       <c r="A80" s="0" t="n">
         <v>79</v>
       </c>
+      <c r="B80" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80" s="0" t="n">
+        <v>25.984</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="81">
       <c r="A81" s="0" t="n">
         <v>80</v>
       </c>
+      <c r="B81" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C81" s="0" t="n">
+        <v>25.272</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="82">
       <c r="A82" s="0" t="n">
         <v>81</v>
       </c>
+      <c r="B82" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" s="0" t="n">
+        <v>25.123</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="83">
       <c r="A83" s="0" t="n">
         <v>82</v>
       </c>
+      <c r="B83" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C83" s="0" t="n">
+        <v>24.933</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="84">
       <c r="A84" s="0" t="n">
         <v>83</v>
       </c>
+      <c r="B84" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C84" s="0" t="n">
+        <v>24.763</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="85">
       <c r="A85" s="0" t="n">
         <v>84</v>
       </c>
+      <c r="B85" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C85" s="0" t="n">
+        <v>24.755</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="86">
       <c r="A86" s="0" t="n">
         <v>85</v>
       </c>
+      <c r="B86" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C86" s="0" t="n">
+        <v>24.174</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="87">
       <c r="A87" s="0" t="n">
         <v>86</v>
       </c>
+      <c r="B87" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C87" s="0" t="n">
+        <v>26.222</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="88">
       <c r="A88" s="0" t="n">
         <v>87</v>
       </c>
+      <c r="B88" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C88" s="0" t="n">
+        <v>24.266</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="89">
       <c r="A89" s="0" t="n">
         <v>88</v>
       </c>
+      <c r="B89" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C89" s="0" t="n">
+        <v>24.738</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="90">
       <c r="A90" s="0" t="n">
         <v>89</v>
       </c>
+      <c r="B90" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C90" s="0" t="n">
+        <v>26.535</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="91">
       <c r="A91" s="0" t="n">
         <v>90</v>
       </c>
+      <c r="B91" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C91" s="0" t="n">
+        <v>24.378</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="92">
       <c r="A92" s="0" t="n">
         <v>91</v>
       </c>
+      <c r="B92" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C92" s="0" t="n">
+        <v>23.956</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="93">
       <c r="A93" s="0" t="n">
         <v>92</v>
       </c>
+      <c r="B93" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C93" s="0" t="n">
+        <v>24.514</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="94">
       <c r="A94" s="0" t="n">
         <v>93</v>
       </c>
+      <c r="B94" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C94" s="0" t="n">
+        <v>24.209</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="95">
       <c r="A95" s="0" t="n">
         <v>94</v>
       </c>
+      <c r="B95" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C95" s="0" t="n">
+        <v>24.683</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="96">
       <c r="A96" s="0" t="n">
         <v>95</v>
       </c>
+      <c r="B96" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C96" s="0" t="n">
+        <v>24.86</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="97">
       <c r="A97" s="0" t="n">
         <v>96</v>
       </c>
+      <c r="B97" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C97" s="0" t="n">
+        <v>26.325</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="98">
       <c r="A98" s="0" t="n">
         <v>97</v>
       </c>
+      <c r="B98" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C98" s="0" t="n">
+        <v>25.655</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="99">
       <c r="A99" s="0" t="n">
         <v>98</v>
       </c>
+      <c r="B99" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C99" s="0" t="n">
+        <v>25.613</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="100">
       <c r="A100" s="0" t="n">
         <v>99</v>
       </c>
+      <c r="B100" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C100" s="0" t="n">
+        <v>25.682</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="101">
       <c r="A101" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="B101" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C101" s="0" t="n">
+        <v>25.171</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="102">
       <c r="A102" s="0" t="n">
         <v>101</v>
       </c>
+      <c r="B102" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C102" s="0" t="n">
+        <v>26.326</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="103">
       <c r="A103" s="0" t="n">
         <v>102</v>
       </c>
+      <c r="B103" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C103" s="0" t="n">
+        <v>24.733</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="104">
       <c r="A104" s="0" t="n">
         <v>103</v>
       </c>
+      <c r="B104" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C104" s="0" t="n">
+        <v>24.322</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="105">
       <c r="A105" s="0" t="n">
         <v>104</v>
       </c>
+      <c r="B105" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C105" s="0" t="n">
+        <v>24.324</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="106">
       <c r="A106" s="0" t="n">
         <v>105</v>
       </c>
+      <c r="B106" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C106" s="0" t="n">
+        <v>26.312</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="107">
       <c r="A107" s="0" t="n">
         <v>106</v>
       </c>
+      <c r="B107" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C107" s="0" t="n">
+        <v>25.133</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="108">
       <c r="A108" s="0" t="n">
         <v>107</v>
       </c>
+      <c r="B108" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C108" s="0" t="n">
+        <v>25.254</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="109">
       <c r="A109" s="0" t="n">
         <v>108</v>
       </c>
+      <c r="B109" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C109" s="0" t="n">
+        <v>24.744</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="110">
       <c r="A110" s="0" t="n">
         <v>109</v>
       </c>
+      <c r="B110" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C110" s="0" t="n">
+        <v>25.47</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="111">
       <c r="A111" s="0" t="n">
         <v>110</v>
       </c>
+      <c r="B111" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C111" s="0" t="n">
+        <v>24.589</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="112">
       <c r="A112" s="0" t="n">
         <v>111</v>
       </c>
+      <c r="B112" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C112" s="0" t="n">
+        <v>25.282</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="113">
       <c r="A113" s="0" t="n">
         <v>112</v>
       </c>
+      <c r="B113" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C113" s="0" t="n">
+        <v>25.366</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="114">
       <c r="A114" s="0" t="n">
         <v>113</v>
       </c>
+      <c r="B114" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C114" s="0" t="n">
+        <v>24.524</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="115">
       <c r="A115" s="0" t="n">
         <v>114</v>
       </c>
+      <c r="B115" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C115" s="0" t="n">
+        <v>25.837</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="116">
       <c r="A116" s="0" t="n">
         <v>115</v>
       </c>
+      <c r="B116" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C116" s="0" t="n">
+        <v>26.575</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="117">
       <c r="A117" s="0" t="n">
         <v>116</v>
       </c>
+      <c r="B117" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C117" s="0" t="n">
+        <v>24.911</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="118">
       <c r="A118" s="0" t="n">
         <v>117</v>
       </c>
+      <c r="B118" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C118" s="0" t="n">
+        <v>25.315</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="119">
       <c r="A119" s="0" t="n">
         <v>118</v>
       </c>
+      <c r="B119" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C119" s="0" t="n">
+        <v>24.916</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="120">
       <c r="A120" s="0" t="n">
         <v>119</v>
       </c>
+      <c r="B120" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C120" s="0" t="n">
+        <v>26.437</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="121">
       <c r="A121" s="0" t="n">
         <v>120</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C121" s="0" t="n">
+        <v>26.51</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="122">
@@ -10515,7 +11934,7 @@
   </sheetPr>
   <dimension ref="A1:C188"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A148" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="I23" activeCellId="0" pane="topLeft" sqref="I23"/>
     </sheetView>
   </sheetViews>
@@ -15134,7 +16553,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>21.714</v>
@@ -15183,7 +16602,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>21.748</v>
@@ -15232,7 +16651,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>21.823</v>
@@ -15281,7 +16700,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>21.965</v>
@@ -15330,7 +16749,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>22.573</v>
@@ -15379,7 +16798,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>22.634</v>
@@ -15428,7 +16847,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>23.725</v>

</xml_diff>

<commit_message>
updating Cn fullerene data
</commit_message>
<xml_diff>
--- a/sknano/data/fullerenes/Cn_fullerenes.xlsx
+++ b/sknano/data/fullerenes/Cn_fullerenes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="13" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="875" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="14" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="875" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="C20" sheetId="1" state="visible" r:id="rId2"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="25">
   <si>
     <t>#</t>
   </si>
@@ -3617,8 +3617,8 @@
   </sheetPr>
   <dimension ref="A1:C200"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A89" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B122" activeCellId="0" pane="topLeft" sqref="B122"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B201" activeCellId="0" pane="topLeft" sqref="B201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4957,399 +4957,873 @@
         <v>26.51</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="122">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="122">
       <c r="A122" s="0" t="n">
         <v>121</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C122" s="0" t="n">
+        <v>25.257</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="123">
       <c r="A123" s="0" t="n">
         <v>122</v>
       </c>
+      <c r="B123" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C123" s="0" t="n">
+        <v>26.92</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="124">
       <c r="A124" s="0" t="n">
         <v>123</v>
       </c>
+      <c r="B124" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C124" s="0" t="n">
+        <v>26.905</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="125">
       <c r="A125" s="0" t="n">
         <v>124</v>
       </c>
+      <c r="B125" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C125" s="0" t="n">
+        <v>24.697</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="126">
       <c r="A126" s="0" t="n">
         <v>125</v>
       </c>
+      <c r="B126" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C126" s="0" t="n">
+        <v>25.085</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="127">
       <c r="A127" s="0" t="n">
         <v>126</v>
       </c>
+      <c r="B127" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C127" s="0" t="n">
+        <v>24.594</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="128">
       <c r="A128" s="0" t="n">
         <v>127</v>
       </c>
+      <c r="B128" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C128" s="0" t="n">
+        <v>24.052</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="129">
       <c r="A129" s="0" t="n">
         <v>128</v>
       </c>
+      <c r="B129" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C129" s="0" t="n">
+        <v>24.637</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="130">
       <c r="A130" s="0" t="n">
         <v>129</v>
       </c>
+      <c r="B130" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C130" s="0" t="n">
+        <v>24.642</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="131">
       <c r="A131" s="0" t="n">
         <v>130</v>
       </c>
+      <c r="B131" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C131" s="0" t="n">
+        <v>24.793</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="132">
       <c r="A132" s="0" t="n">
         <v>131</v>
       </c>
+      <c r="B132" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C132" s="0" t="n">
+        <v>24.639</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="133">
       <c r="A133" s="0" t="n">
         <v>132</v>
       </c>
+      <c r="B133" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C133" s="0" t="n">
+        <v>25.68</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="134">
       <c r="A134" s="0" t="n">
         <v>133</v>
       </c>
+      <c r="B134" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C134" s="0" t="n">
+        <v>24.258</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="135">
       <c r="A135" s="0" t="n">
         <v>134</v>
       </c>
+      <c r="B135" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C135" s="0" t="n">
+        <v>25.66</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="136">
       <c r="A136" s="0" t="n">
         <v>135</v>
       </c>
+      <c r="B136" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C136" s="0" t="n">
+        <v>23.629</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="137">
       <c r="A137" s="0" t="n">
         <v>136</v>
       </c>
+      <c r="B137" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C137" s="0" t="n">
+        <v>25.144</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="138">
       <c r="A138" s="0" t="n">
         <v>137</v>
       </c>
+      <c r="B138" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C138" s="0" t="n">
+        <v>23.48</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="139">
       <c r="A139" s="0" t="n">
         <v>138</v>
       </c>
+      <c r="B139" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C139" s="0" t="n">
+        <v>23.526</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="140">
       <c r="A140" s="0" t="n">
         <v>139</v>
       </c>
+      <c r="B140" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C140" s="0" t="n">
+        <v>23.171</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="141">
       <c r="A141" s="0" t="n">
         <v>140</v>
       </c>
+      <c r="B141" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C141" s="0" t="n">
+        <v>23.351</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="142">
       <c r="A142" s="0" t="n">
         <v>141</v>
       </c>
+      <c r="B142" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C142" s="0" t="n">
+        <v>24.086</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="143">
       <c r="A143" s="0" t="n">
         <v>142</v>
       </c>
+      <c r="B143" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C143" s="0" t="n">
+        <v>24.077</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="144">
       <c r="A144" s="0" t="n">
         <v>143</v>
       </c>
+      <c r="B144" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C144" s="0" t="n">
+        <v>25.055</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="145">
       <c r="A145" s="0" t="n">
         <v>144</v>
       </c>
+      <c r="B145" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C145" s="0" t="n">
+        <v>26.824</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="146">
       <c r="A146" s="0" t="n">
         <v>145</v>
       </c>
+      <c r="B146" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C146" s="0" t="n">
+        <v>23.52</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="147">
       <c r="A147" s="0" t="n">
         <v>146</v>
       </c>
+      <c r="B147" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C147" s="0" t="n">
+        <v>24.162</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="148">
       <c r="A148" s="0" t="n">
         <v>147</v>
       </c>
+      <c r="B148" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C148" s="0" t="n">
+        <v>23.756</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="149">
       <c r="A149" s="0" t="n">
         <v>148</v>
       </c>
+      <c r="B149" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C149" s="0" t="n">
+        <v>23.347</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="150">
       <c r="A150" s="0" t="n">
         <v>149</v>
       </c>
+      <c r="B150" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C150" s="0" t="n">
+        <v>22.944</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="151">
       <c r="A151" s="0" t="n">
         <v>150</v>
       </c>
+      <c r="B151" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C151" s="0" t="n">
+        <v>23.231</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="152">
       <c r="A152" s="0" t="n">
         <v>151</v>
       </c>
+      <c r="B152" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C152" s="0" t="n">
+        <v>23.839</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="153">
       <c r="A153" s="0" t="n">
         <v>152</v>
       </c>
+      <c r="B153" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C153" s="0" t="n">
+        <v>24.375</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="154">
       <c r="A154" s="0" t="n">
         <v>153</v>
       </c>
+      <c r="B154" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C154" s="0" t="n">
+        <v>24.445</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="155">
       <c r="A155" s="0" t="n">
         <v>154</v>
       </c>
+      <c r="B155" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C155" s="0" t="n">
+        <v>24.044</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="156">
       <c r="A156" s="0" t="n">
         <v>155</v>
       </c>
+      <c r="B156" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C156" s="0" t="n">
+        <v>23.56</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="157">
       <c r="A157" s="0" t="n">
         <v>156</v>
       </c>
+      <c r="B157" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C157" s="0" t="n">
+        <v>23.483</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="158">
       <c r="A158" s="0" t="n">
         <v>157</v>
       </c>
+      <c r="B158" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C158" s="0" t="n">
+        <v>25.159</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="159">
       <c r="A159" s="0" t="n">
         <v>158</v>
       </c>
+      <c r="B159" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C159" s="0" t="n">
+        <v>23.965</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="160">
       <c r="A160" s="0" t="n">
         <v>159</v>
       </c>
+      <c r="B160" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C160" s="0" t="n">
+        <v>23.999</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="161">
       <c r="A161" s="0" t="n">
         <v>160</v>
       </c>
+      <c r="B161" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C161" s="0" t="n">
+        <v>23.765</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="162">
       <c r="A162" s="0" t="n">
         <v>161</v>
       </c>
+      <c r="B162" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C162" s="0" t="n">
+        <v>23.833</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="163">
       <c r="A163" s="0" t="n">
         <v>162</v>
       </c>
+      <c r="B163" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C163" s="0" t="n">
+        <v>23.543</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="164">
       <c r="A164" s="0" t="n">
         <v>163</v>
       </c>
+      <c r="B164" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C164" s="0" t="n">
+        <v>23.132</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="165">
       <c r="A165" s="0" t="n">
         <v>164</v>
       </c>
+      <c r="B165" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C165" s="0" t="n">
+        <v>23.948</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="166">
       <c r="A166" s="0" t="n">
         <v>165</v>
       </c>
+      <c r="B166" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C166" s="0" t="n">
+        <v>22.927</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="167">
       <c r="A167" s="0" t="n">
         <v>166</v>
       </c>
+      <c r="B167" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C167" s="0" t="n">
+        <v>23.565</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="168">
       <c r="A168" s="0" t="n">
         <v>167</v>
       </c>
+      <c r="B168" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C168" s="0" t="n">
+        <v>23.288</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="169">
       <c r="A169" s="0" t="n">
         <v>168</v>
       </c>
+      <c r="B169" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C169" s="0" t="n">
+        <v>23.487</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="170">
       <c r="A170" s="0" t="n">
         <v>169</v>
       </c>
+      <c r="B170" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C170" s="0" t="n">
+        <v>23.276</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="171">
       <c r="A171" s="0" t="n">
         <v>170</v>
       </c>
+      <c r="B171" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C171" s="0" t="n">
+        <v>22.624</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="172">
       <c r="A172" s="0" t="n">
         <v>171</v>
       </c>
+      <c r="B172" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C172" s="0" t="n">
+        <v>23.101</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="173">
       <c r="A173" s="0" t="n">
         <v>172</v>
       </c>
+      <c r="B173" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C173" s="0" t="n">
+        <v>24.645</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="174">
       <c r="A174" s="0" t="n">
         <v>173</v>
       </c>
+      <c r="B174" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C174" s="0" t="n">
+        <v>23.688</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="175">
       <c r="A175" s="0" t="n">
         <v>174</v>
       </c>
+      <c r="B175" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C175" s="0" t="n">
+        <v>24.792</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="176">
       <c r="A176" s="0" t="n">
         <v>175</v>
       </c>
+      <c r="B176" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C176" s="0" t="n">
+        <v>24.138</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="177">
       <c r="A177" s="0" t="n">
         <v>176</v>
       </c>
+      <c r="B177" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C177" s="0" t="n">
+        <v>23.717</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="178">
       <c r="A178" s="0" t="n">
         <v>177</v>
       </c>
+      <c r="B178" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C178" s="0" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="179">
       <c r="A179" s="0" t="n">
         <v>178</v>
       </c>
+      <c r="B179" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C179" s="0" t="n">
+        <v>23.628</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="180">
       <c r="A180" s="0" t="n">
         <v>179</v>
       </c>
+      <c r="B180" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C180" s="0" t="n">
+        <v>24.1</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="181">
       <c r="A181" s="0" t="n">
         <v>180</v>
       </c>
+      <c r="B181" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C181" s="0" t="n">
+        <v>24.037</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="182">
       <c r="A182" s="0" t="n">
         <v>181</v>
       </c>
+      <c r="B182" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C182" s="0" t="n">
+        <v>25.528</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="183">
       <c r="A183" s="0" t="n">
         <v>182</v>
       </c>
+      <c r="B183" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C183" s="0" t="n">
+        <v>25.046</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="184">
       <c r="A184" s="0" t="n">
         <v>183</v>
       </c>
+      <c r="B184" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C184" s="0" t="n">
+        <v>23.468</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="185">
       <c r="A185" s="0" t="n">
         <v>184</v>
       </c>
+      <c r="B185" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C185" s="0" t="n">
+        <v>24.292</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="186">
       <c r="A186" s="0" t="n">
         <v>185</v>
       </c>
+      <c r="B186" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C186" s="0" t="n">
+        <v>23.381</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="187">
       <c r="A187" s="0" t="n">
         <v>186</v>
       </c>
+      <c r="B187" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C187" s="0" t="n">
+        <v>26.953</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="188">
       <c r="A188" s="0" t="n">
         <v>187</v>
       </c>
+      <c r="B188" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C188" s="0" t="n">
+        <v>23.245</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="189">
       <c r="A189" s="0" t="n">
         <v>188</v>
       </c>
+      <c r="B189" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C189" s="0" t="n">
+        <v>22.993</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="190">
       <c r="A190" s="0" t="n">
         <v>189</v>
       </c>
+      <c r="B190" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C190" s="0" t="n">
+        <v>26.643</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="191">
       <c r="A191" s="0" t="n">
         <v>190</v>
       </c>
+      <c r="B191" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C191" s="0" t="n">
+        <v>24.979</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="192">
       <c r="A192" s="0" t="n">
         <v>191</v>
       </c>
+      <c r="B192" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C192" s="0" t="n">
+        <v>24.796</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="193">
       <c r="A193" s="0" t="n">
         <v>192</v>
       </c>
+      <c r="B193" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C193" s="0" t="n">
+        <v>23.096</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="194">
       <c r="A194" s="0" t="n">
         <v>193</v>
       </c>
+      <c r="B194" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C194" s="0" t="n">
+        <v>23.436</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="195">
       <c r="A195" s="0" t="n">
         <v>194</v>
       </c>
+      <c r="B195" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C195" s="0" t="n">
+        <v>23.104</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="196">
       <c r="A196" s="0" t="n">
         <v>195</v>
       </c>
+      <c r="B196" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C196" s="0" t="n">
+        <v>22.944</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="197">
       <c r="A197" s="0" t="n">
         <v>196</v>
       </c>
+      <c r="B197" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C197" s="0" t="n">
+        <v>24.718</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="198">
       <c r="A198" s="0" t="n">
         <v>197</v>
       </c>
+      <c r="B198" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C198" s="0" t="n">
+        <v>22.946</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="199">
       <c r="A199" s="0" t="n">
         <v>198</v>
       </c>
+      <c r="B199" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C199" s="0" t="n">
+        <v>23.815</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="200">
       <c r="A200" s="0" t="n">
         <v>199</v>
+      </c>
+      <c r="B200" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C200" s="0" t="n">
+        <v>22.376</v>
       </c>
     </row>
   </sheetData>
@@ -5370,8 +5844,8 @@
   </sheetPr>
   <dimension ref="A1:C272"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B10" activeCellId="0" pane="topLeft" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5394,40 +5868,88 @@
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="B2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>34.883</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="3">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="B3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>31.919</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="4">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="B4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>35.747</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="5">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="B5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>28.936</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="6">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="B6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>29.08</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="7">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="B7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>30.333</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="8">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="B8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>29.243</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="9">
       <c r="A9" s="0" t="n">
         <v>8</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>28.39</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="10">

</xml_diff>

<commit_message>
adding more fullerene data to spreadsheet
</commit_message>
<xml_diff>
--- a/sknano/data/fullerenes/Cn_fullerenes.xlsx
+++ b/sknano/data/fullerenes/Cn_fullerenes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="14" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="875" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="14" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="799" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="C20" sheetId="1" state="visible" r:id="rId2"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="25">
   <si>
     <t>#</t>
   </si>
@@ -5844,8 +5844,8 @@
   </sheetPr>
   <dimension ref="A1:C272"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B10" activeCellId="0" pane="topLeft" sqref="B10"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A154" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B202" activeCellId="0" pane="topLeft" sqref="B202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5952,964 +5952,2116 @@
         <v>28.39</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
+      <c r="B10" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>28.216</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="11">
       <c r="A11" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>29.848</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="12">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
+      <c r="B12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>29.774</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="13">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
+      <c r="B13" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>28.626</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="14">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
+      <c r="B14" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>32.622</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="15">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
+      <c r="B15" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>28.986</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="16">
       <c r="A16" s="0" t="n">
         <v>15</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>29.092</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="17">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="B17" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>29.659</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="18">
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
+      <c r="B18" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>29.101</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="19">
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
+      <c r="B19" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>30.016</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="20">
       <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
+      <c r="B20" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>27.725</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="21">
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="B21" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>27.182</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="22">
       <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
+      <c r="B22" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>27.308</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="23">
       <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
+      <c r="B23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>28.08</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="24">
       <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
+      <c r="B24" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>26.886</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="25">
       <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
+      <c r="B25" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>28.144</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="26">
       <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
+      <c r="B26" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>27.939</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="27">
       <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
+      <c r="B27" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>27.968</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="28">
       <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
+      <c r="B28" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>27.259</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="29">
       <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
+      <c r="B29" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>28.574</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="30">
       <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
+      <c r="B30" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>26.524</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="31">
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="B31" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>26.677</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="32">
       <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
+      <c r="B32" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>26.274</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="33">
       <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="B33" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>27.005</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="34">
       <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
+      <c r="B34" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>26.837</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="35">
       <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
+      <c r="B35" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>26.893</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="36">
       <c r="A36" s="0" t="n">
         <v>35</v>
       </c>
+      <c r="B36" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>26.741</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="37">
       <c r="A37" s="0" t="n">
         <v>36</v>
       </c>
+      <c r="B37" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>27.059</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="38">
       <c r="A38" s="0" t="n">
         <v>37</v>
       </c>
+      <c r="B38" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>26.383</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="39">
       <c r="A39" s="0" t="n">
         <v>38</v>
       </c>
+      <c r="B39" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>27.265</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="40">
       <c r="A40" s="0" t="n">
         <v>39</v>
       </c>
+      <c r="B40" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>25.623</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="41">
       <c r="A41" s="0" t="n">
         <v>40</v>
       </c>
+      <c r="B41" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>25.557</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="42">
       <c r="A42" s="0" t="n">
         <v>41</v>
       </c>
+      <c r="B42" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>26.809</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="43">
       <c r="A43" s="0" t="n">
         <v>42</v>
       </c>
+      <c r="B43" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>25.409</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="44">
       <c r="A44" s="0" t="n">
         <v>43</v>
       </c>
+      <c r="B44" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>26.414</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="45">
       <c r="A45" s="0" t="n">
         <v>44</v>
       </c>
+      <c r="B45" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>24.254</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="46">
       <c r="A46" s="0" t="n">
         <v>45</v>
       </c>
+      <c r="B46" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>27.171</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="47">
       <c r="A47" s="0" t="n">
         <v>46</v>
       </c>
+      <c r="B47" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>26.707</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="48">
       <c r="A48" s="0" t="n">
         <v>47</v>
       </c>
+      <c r="B48" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>25.71</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="49">
       <c r="A49" s="0" t="n">
         <v>48</v>
       </c>
+      <c r="B49" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>26.625</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="50">
       <c r="A50" s="0" t="n">
         <v>49</v>
       </c>
+      <c r="B50" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>25.523</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="51">
       <c r="A51" s="0" t="n">
         <v>50</v>
       </c>
+      <c r="B51" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>27.012</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="52">
       <c r="A52" s="0" t="n">
         <v>51</v>
       </c>
+      <c r="B52" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>25.541</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="53">
       <c r="A53" s="0" t="n">
         <v>52</v>
       </c>
+      <c r="B53" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>25.149</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="54">
       <c r="A54" s="0" t="n">
         <v>53</v>
       </c>
+      <c r="B54" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>26.017</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="55">
       <c r="A55" s="0" t="n">
         <v>54</v>
       </c>
+      <c r="B55" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>25.537</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="56">
       <c r="A56" s="0" t="n">
         <v>55</v>
       </c>
+      <c r="B56" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>25.252</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="57">
       <c r="A57" s="0" t="n">
         <v>56</v>
       </c>
+      <c r="B57" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>29.391</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="58">
       <c r="A58" s="0" t="n">
         <v>57</v>
       </c>
+      <c r="B58" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>25.534</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="59">
       <c r="A59" s="0" t="n">
         <v>58</v>
       </c>
+      <c r="B59" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>25.753</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="60">
       <c r="A60" s="0" t="n">
         <v>59</v>
       </c>
+      <c r="B60" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>30.24</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="61">
       <c r="A61" s="0" t="n">
         <v>60</v>
       </c>
+      <c r="B61" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>28.401</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="62">
       <c r="A62" s="0" t="n">
         <v>61</v>
       </c>
+      <c r="B62" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>28.361</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="63">
       <c r="A63" s="0" t="n">
         <v>62</v>
       </c>
+      <c r="B63" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C63" s="0" t="n">
+        <v>25.875</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="64">
       <c r="A64" s="0" t="n">
         <v>63</v>
       </c>
+      <c r="B64" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>26.806</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="65">
       <c r="A65" s="0" t="n">
         <v>64</v>
       </c>
+      <c r="B65" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>27.497</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="66">
       <c r="A66" s="0" t="n">
         <v>65</v>
       </c>
+      <c r="B66" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <v>26.227</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="67">
       <c r="A67" s="0" t="n">
         <v>66</v>
       </c>
+      <c r="B67" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" s="0" t="n">
+        <v>26.594</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="68">
       <c r="A68" s="0" t="n">
         <v>67</v>
       </c>
+      <c r="B68" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C68" s="0" t="n">
+        <v>27.783</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="69">
       <c r="A69" s="0" t="n">
         <v>68</v>
       </c>
+      <c r="B69" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C69" s="0" t="n">
+        <v>25.8</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="70">
       <c r="A70" s="0" t="n">
         <v>69</v>
       </c>
+      <c r="B70" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C70" s="0" t="n">
+        <v>25.369</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="71">
       <c r="A71" s="0" t="n">
         <v>70</v>
       </c>
+      <c r="B71" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" s="0" t="n">
+        <v>25.501</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="72">
       <c r="A72" s="0" t="n">
         <v>71</v>
       </c>
+      <c r="B72" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C72" s="0" t="n">
+        <v>27.783</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="73">
       <c r="A73" s="0" t="n">
         <v>72</v>
       </c>
+      <c r="B73" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C73" s="0" t="n">
+        <v>26.034</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="74">
       <c r="A74" s="0" t="n">
         <v>73</v>
       </c>
+      <c r="B74" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C74" s="0" t="n">
+        <v>26.938</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="75">
       <c r="A75" s="0" t="n">
         <v>74</v>
       </c>
+      <c r="B75" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C75" s="0" t="n">
+        <v>26.73</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="76">
       <c r="A76" s="0" t="n">
         <v>75</v>
       </c>
+      <c r="B76" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C76" s="0" t="n">
+        <v>26.376</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="77">
       <c r="A77" s="0" t="n">
         <v>76</v>
       </c>
+      <c r="B77" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C77" s="0" t="n">
+        <v>26.949</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="78">
       <c r="A78" s="0" t="n">
         <v>77</v>
       </c>
+      <c r="B78" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C78" s="0" t="n">
+        <v>26.327</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="79">
       <c r="A79" s="0" t="n">
         <v>78</v>
       </c>
+      <c r="B79" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C79" s="0" t="n">
+        <v>27.894</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="80">
       <c r="A80" s="0" t="n">
         <v>79</v>
       </c>
+      <c r="B80" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80" s="0" t="n">
+        <v>27.873</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="81">
       <c r="A81" s="0" t="n">
         <v>80</v>
       </c>
+      <c r="B81" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C81" s="0" t="n">
+        <v>27.815</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="82">
       <c r="A82" s="0" t="n">
         <v>81</v>
       </c>
+      <c r="B82" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C82" s="0" t="n">
+        <v>26.611</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="83">
       <c r="A83" s="0" t="n">
         <v>82</v>
       </c>
+      <c r="B83" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C83" s="0" t="n">
+        <v>25.64</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="84">
       <c r="A84" s="0" t="n">
         <v>83</v>
       </c>
+      <c r="B84" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C84" s="0" t="n">
+        <v>25.279</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="85">
       <c r="A85" s="0" t="n">
         <v>84</v>
       </c>
+      <c r="B85" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C85" s="0" t="n">
+        <v>26.596</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="86">
       <c r="A86" s="0" t="n">
         <v>85</v>
       </c>
+      <c r="B86" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C86" s="0" t="n">
+        <v>25.717</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="87">
       <c r="A87" s="0" t="n">
         <v>86</v>
       </c>
+      <c r="B87" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C87" s="0" t="n">
+        <v>27.351</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="88">
       <c r="A88" s="0" t="n">
         <v>87</v>
       </c>
+      <c r="B88" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C88" s="0" t="n">
+        <v>26.083</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="89">
       <c r="A89" s="0" t="n">
         <v>88</v>
       </c>
+      <c r="B89" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C89" s="0" t="n">
+        <v>25.345</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="90">
       <c r="A90" s="0" t="n">
         <v>89</v>
       </c>
+      <c r="B90" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C90" s="0" t="n">
+        <v>26.873</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="91">
       <c r="A91" s="0" t="n">
         <v>90</v>
       </c>
+      <c r="B91" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C91" s="0" t="n">
+        <v>26.257</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="92">
       <c r="A92" s="0" t="n">
         <v>91</v>
       </c>
+      <c r="B92" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C92" s="0" t="n">
+        <v>25.234</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="93">
       <c r="A93" s="0" t="n">
         <v>92</v>
       </c>
+      <c r="B93" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C93" s="0" t="n">
+        <v>26.354</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="94">
       <c r="A94" s="0" t="n">
         <v>93</v>
       </c>
+      <c r="B94" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C94" s="0" t="n">
+        <v>27.309</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="95">
       <c r="A95" s="0" t="n">
         <v>94</v>
       </c>
+      <c r="B95" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C95" s="0" t="n">
+        <v>26.629</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="96">
       <c r="A96" s="0" t="n">
         <v>95</v>
       </c>
+      <c r="B96" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C96" s="0" t="n">
+        <v>25.919</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="97">
       <c r="A97" s="0" t="n">
         <v>96</v>
       </c>
+      <c r="B97" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C97" s="0" t="n">
+        <v>25.813</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="98">
       <c r="A98" s="0" t="n">
         <v>97</v>
       </c>
+      <c r="B98" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C98" s="0" t="n">
+        <v>25.176</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="99">
       <c r="A99" s="0" t="n">
         <v>98</v>
       </c>
+      <c r="B99" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C99" s="0" t="n">
+        <v>24.893</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="100">
       <c r="A100" s="0" t="n">
         <v>99</v>
       </c>
+      <c r="B100" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C100" s="0" t="n">
+        <v>24.992</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="101">
       <c r="A101" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="B101" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C101" s="0" t="n">
+        <v>24.873</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="102">
       <c r="A102" s="0" t="n">
         <v>101</v>
       </c>
+      <c r="B102" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C102" s="0" t="n">
+        <v>25.125</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="103">
       <c r="A103" s="0" t="n">
         <v>102</v>
       </c>
+      <c r="B103" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C103" s="0" t="n">
+        <v>24.462</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="104">
       <c r="A104" s="0" t="n">
         <v>103</v>
       </c>
+      <c r="B104" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C104" s="0" t="n">
+        <v>25.7</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="105">
       <c r="A105" s="0" t="n">
         <v>104</v>
       </c>
+      <c r="B105" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C105" s="0" t="n">
+        <v>24.646</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="106">
       <c r="A106" s="0" t="n">
         <v>105</v>
       </c>
+      <c r="B106" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C106" s="0" t="n">
+        <v>25.118</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="107">
       <c r="A107" s="0" t="n">
         <v>106</v>
       </c>
+      <c r="B107" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C107" s="0" t="n">
+        <v>24.968</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="108">
       <c r="A108" s="0" t="n">
         <v>107</v>
       </c>
+      <c r="B108" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C108" s="0" t="n">
+        <v>24.179</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="109">
       <c r="A109" s="0" t="n">
         <v>108</v>
       </c>
+      <c r="B109" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C109" s="0" t="n">
+        <v>25.171</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="110">
       <c r="A110" s="0" t="n">
         <v>109</v>
       </c>
+      <c r="B110" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C110" s="0" t="n">
+        <v>24.94</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="111">
       <c r="A111" s="0" t="n">
         <v>110</v>
       </c>
+      <c r="B111" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C111" s="0" t="n">
+        <v>24.752</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="112">
       <c r="A112" s="0" t="n">
         <v>111</v>
       </c>
+      <c r="B112" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C112" s="0" t="n">
+        <v>24.314</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="113">
       <c r="A113" s="0" t="n">
         <v>112</v>
       </c>
+      <c r="B113" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C113" s="0" t="n">
+        <v>25.247</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="114">
       <c r="A114" s="0" t="n">
         <v>113</v>
       </c>
+      <c r="B114" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C114" s="0" t="n">
+        <v>24.973</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="115">
       <c r="A115" s="0" t="n">
         <v>114</v>
       </c>
+      <c r="B115" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C115" s="0" t="n">
+        <v>24.398</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="116">
       <c r="A116" s="0" t="n">
         <v>115</v>
       </c>
+      <c r="B116" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C116" s="0" t="n">
+        <v>24.085</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="117">
       <c r="A117" s="0" t="n">
         <v>116</v>
       </c>
+      <c r="B117" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C117" s="0" t="n">
+        <v>26.571</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="118">
       <c r="A118" s="0" t="n">
         <v>117</v>
       </c>
+      <c r="B118" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C118" s="0" t="n">
+        <v>24.488</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="119">
       <c r="A119" s="0" t="n">
         <v>118</v>
       </c>
+      <c r="B119" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C119" s="0" t="n">
+        <v>24.85</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="120">
       <c r="A120" s="0" t="n">
         <v>119</v>
       </c>
+      <c r="B120" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C120" s="0" t="n">
+        <v>24.514</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="121">
       <c r="A121" s="0" t="n">
         <v>120</v>
       </c>
+      <c r="B121" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C121" s="0" t="n">
+        <v>25.293</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="122">
       <c r="A122" s="0" t="n">
         <v>121</v>
       </c>
+      <c r="B122" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C122" s="0" t="n">
+        <v>25.05</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="123">
       <c r="A123" s="0" t="n">
         <v>122</v>
       </c>
+      <c r="B123" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C123" s="0" t="n">
+        <v>25.583</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="124">
       <c r="A124" s="0" t="n">
         <v>123</v>
       </c>
+      <c r="B124" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C124" s="0" t="n">
+        <v>25.107</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="125">
       <c r="A125" s="0" t="n">
         <v>124</v>
       </c>
+      <c r="B125" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C125" s="0" t="n">
+        <v>25.419</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="126">
       <c r="A126" s="0" t="n">
         <v>125</v>
       </c>
+      <c r="B126" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C126" s="0" t="n">
+        <v>28.328</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="127">
       <c r="A127" s="0" t="n">
         <v>126</v>
       </c>
+      <c r="B127" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C127" s="0" t="n">
+        <v>26.433</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="128">
       <c r="A128" s="0" t="n">
         <v>127</v>
       </c>
+      <c r="B128" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C128" s="0" t="n">
+        <v>25.388</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="129">
       <c r="A129" s="0" t="n">
         <v>128</v>
       </c>
+      <c r="B129" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C129" s="0" t="n">
+        <v>26.236</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="130">
       <c r="A130" s="0" t="n">
         <v>129</v>
       </c>
+      <c r="B130" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C130" s="0" t="n">
+        <v>25.401</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="131">
       <c r="A131" s="0" t="n">
         <v>130</v>
       </c>
+      <c r="B131" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C131" s="0" t="n">
+        <v>25.496</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="132">
       <c r="A132" s="0" t="n">
         <v>131</v>
       </c>
+      <c r="B132" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C132" s="0" t="n">
+        <v>25.835</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="133">
       <c r="A133" s="0" t="n">
         <v>132</v>
       </c>
+      <c r="B133" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C133" s="0" t="n">
+        <v>24.932</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="134">
       <c r="A134" s="0" t="n">
         <v>133</v>
       </c>
+      <c r="B134" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C134" s="0" t="n">
+        <v>25.397</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="135">
       <c r="A135" s="0" t="n">
         <v>134</v>
       </c>
+      <c r="B135" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C135" s="0" t="n">
+        <v>26.498</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="136">
       <c r="A136" s="0" t="n">
         <v>135</v>
       </c>
+      <c r="B136" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C136" s="0" t="n">
+        <v>26.311</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="137">
       <c r="A137" s="0" t="n">
         <v>136</v>
       </c>
+      <c r="B137" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C137" s="0" t="n">
+        <v>26.851</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="138">
       <c r="A138" s="0" t="n">
         <v>137</v>
       </c>
+      <c r="B138" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C138" s="0" t="n">
+        <v>25.558</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="139">
       <c r="A139" s="0" t="n">
         <v>138</v>
       </c>
+      <c r="B139" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C139" s="0" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="140">
       <c r="A140" s="0" t="n">
         <v>139</v>
       </c>
+      <c r="B140" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C140" s="0" t="n">
+        <v>27.209</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="141">
       <c r="A141" s="0" t="n">
         <v>140</v>
       </c>
+      <c r="B141" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C141" s="0" t="n">
+        <v>26.674</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="142">
       <c r="A142" s="0" t="n">
         <v>141</v>
       </c>
+      <c r="B142" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C142" s="0" t="n">
+        <v>27.933</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="143">
       <c r="A143" s="0" t="n">
         <v>142</v>
       </c>
+      <c r="B143" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C143" s="0" t="n">
+        <v>25.914</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="144">
       <c r="A144" s="0" t="n">
         <v>143</v>
       </c>
+      <c r="B144" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C144" s="0" t="n">
+        <v>24.222</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="145">
       <c r="A145" s="0" t="n">
         <v>144</v>
       </c>
+      <c r="B145" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C145" s="0" t="n">
+        <v>24.157</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="146">
       <c r="A146" s="0" t="n">
         <v>145</v>
       </c>
+      <c r="B146" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C146" s="0" t="n">
+        <v>24.588</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="147">
       <c r="A147" s="0" t="n">
         <v>146</v>
       </c>
+      <c r="B147" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C147" s="0" t="n">
+        <v>24.185</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="148">
       <c r="A148" s="0" t="n">
         <v>147</v>
       </c>
+      <c r="B148" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C148" s="0" t="n">
+        <v>25.322</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="149">
       <c r="A149" s="0" t="n">
         <v>148</v>
       </c>
+      <c r="B149" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C149" s="0" t="n">
+        <v>27.548</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="150">
       <c r="A150" s="0" t="n">
         <v>149</v>
       </c>
+      <c r="B150" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C150" s="0" t="n">
+        <v>25.128</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="151">
       <c r="A151" s="0" t="n">
         <v>150</v>
       </c>
+      <c r="B151" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C151" s="0" t="n">
+        <v>24.175</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="152">
       <c r="A152" s="0" t="n">
         <v>151</v>
       </c>
+      <c r="B152" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C152" s="0" t="n">
+        <v>24.418</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="153">
       <c r="A153" s="0" t="n">
         <v>152</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="154">
+      <c r="B153" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C153" s="0" t="n">
+        <v>25.643</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="154">
       <c r="A154" s="0" t="n">
         <v>153</v>
+      </c>
+      <c r="B154" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C154" s="0" t="n">
+        <v>25.038</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="155">
       <c r="A155" s="0" t="n">
         <v>154</v>
       </c>
+      <c r="B155" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C155" s="0" t="n">
+        <v>25.125</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="156">
       <c r="A156" s="0" t="n">
         <v>155</v>
       </c>
+      <c r="B156" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C156" s="0" t="n">
+        <v>26.479</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="157">
       <c r="A157" s="0" t="n">
         <v>156</v>
       </c>
+      <c r="B157" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C157" s="0" t="n">
+        <v>25.427</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="158">
       <c r="A158" s="0" t="n">
         <v>157</v>
       </c>
+      <c r="B158" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C158" s="0" t="n">
+        <v>24.445</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="159">
       <c r="A159" s="0" t="n">
         <v>158</v>
       </c>
+      <c r="B159" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C159" s="0" t="n">
+        <v>24.481</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="160">
       <c r="A160" s="0" t="n">
         <v>159</v>
       </c>
+      <c r="B160" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C160" s="0" t="n">
+        <v>25.427</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="161">
       <c r="A161" s="0" t="n">
         <v>160</v>
       </c>
+      <c r="B161" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C161" s="0" t="n">
+        <v>24.879</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="162">
       <c r="A162" s="0" t="n">
         <v>161</v>
       </c>
+      <c r="B162" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C162" s="0" t="n">
+        <v>26.202</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="163">
       <c r="A163" s="0" t="n">
         <v>162</v>
       </c>
+      <c r="B163" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C163" s="0" t="n">
+        <v>26.156</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="164">
       <c r="A164" s="0" t="n">
         <v>163</v>
       </c>
+      <c r="B164" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C164" s="0" t="n">
+        <v>24.521</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="165">
       <c r="A165" s="0" t="n">
         <v>164</v>
       </c>
+      <c r="B165" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C165" s="0" t="n">
+        <v>26.204</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="166">
       <c r="A166" s="0" t="n">
         <v>165</v>
       </c>
+      <c r="B166" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C166" s="0" t="n">
+        <v>24.755</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="167">
       <c r="A167" s="0" t="n">
         <v>166</v>
       </c>
+      <c r="B167" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C167" s="0" t="n">
+        <v>25.045</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="168">
       <c r="A168" s="0" t="n">
         <v>167</v>
       </c>
+      <c r="B168" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C168" s="0" t="n">
+        <v>24.941</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="169">
       <c r="A169" s="0" t="n">
         <v>168</v>
       </c>
+      <c r="B169" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C169" s="0" t="n">
+        <v>24.603</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="170">
       <c r="A170" s="0" t="n">
         <v>169</v>
       </c>
+      <c r="B170" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C170" s="0" t="n">
+        <v>23.885</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="171">
       <c r="A171" s="0" t="n">
         <v>170</v>
       </c>
+      <c r="B171" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C171" s="0" t="n">
+        <v>25.732</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="172">
       <c r="A172" s="0" t="n">
         <v>171</v>
       </c>
+      <c r="B172" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C172" s="0" t="n">
+        <v>23.93</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="173">
       <c r="A173" s="0" t="n">
         <v>172</v>
       </c>
+      <c r="B173" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C173" s="0" t="n">
+        <v>24.099</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="174">
       <c r="A174" s="0" t="n">
         <v>173</v>
       </c>
+      <c r="B174" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C174" s="0" t="n">
+        <v>23.859</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="175">
       <c r="A175" s="0" t="n">
         <v>174</v>
       </c>
+      <c r="B175" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C175" s="0" t="n">
+        <v>24.032</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="176">
       <c r="A176" s="0" t="n">
         <v>175</v>
       </c>
+      <c r="B176" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C176" s="0" t="n">
+        <v>27.841</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="177">
       <c r="A177" s="0" t="n">
         <v>176</v>
       </c>
+      <c r="B177" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C177" s="0" t="n">
+        <v>25.555</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="178">
       <c r="A178" s="0" t="n">
         <v>177</v>
       </c>
+      <c r="B178" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C178" s="0" t="n">
+        <v>24.264</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="179">
       <c r="A179" s="0" t="n">
         <v>178</v>
       </c>
+      <c r="B179" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C179" s="0" t="n">
+        <v>25.516</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="180">
       <c r="A180" s="0" t="n">
         <v>179</v>
       </c>
+      <c r="B180" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C180" s="0" t="n">
+        <v>24.454</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="181">
       <c r="A181" s="0" t="n">
         <v>180</v>
       </c>
+      <c r="B181" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C181" s="0" t="n">
+        <v>26.164</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="182">
       <c r="A182" s="0" t="n">
         <v>181</v>
       </c>
+      <c r="B182" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C182" s="0" t="n">
+        <v>23.7</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="183">
       <c r="A183" s="0" t="n">
         <v>182</v>
       </c>
+      <c r="B183" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C183" s="0" t="n">
+        <v>23.35</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="184">
       <c r="A184" s="0" t="n">
         <v>183</v>
       </c>
+      <c r="B184" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C184" s="0" t="n">
+        <v>23.335</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="185">
       <c r="A185" s="0" t="n">
         <v>184</v>
       </c>
+      <c r="B185" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C185" s="0" t="n">
+        <v>23.605</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="186">
       <c r="A186" s="0" t="n">
         <v>185</v>
       </c>
+      <c r="B186" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C186" s="0" t="n">
+        <v>24.692</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="187">
       <c r="A187" s="0" t="n">
         <v>186</v>
       </c>
+      <c r="B187" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C187" s="0" t="n">
+        <v>24.163</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="188">
       <c r="A188" s="0" t="n">
         <v>187</v>
       </c>
+      <c r="B188" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C188" s="0" t="n">
+        <v>23.748</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="189">
       <c r="A189" s="0" t="n">
         <v>188</v>
       </c>
+      <c r="B189" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C189" s="0" t="n">
+        <v>23.278</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="190">
       <c r="A190" s="0" t="n">
         <v>189</v>
       </c>
+      <c r="B190" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C190" s="0" t="n">
+        <v>23.899</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="191">
       <c r="A191" s="0" t="n">
         <v>190</v>
       </c>
+      <c r="B191" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C191" s="0" t="n">
+        <v>24.972</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="192">
       <c r="A192" s="0" t="n">
         <v>191</v>
       </c>
+      <c r="B192" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C192" s="0" t="n">
+        <v>24.601</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="193">
       <c r="A193" s="0" t="n">
         <v>192</v>
       </c>
+      <c r="B193" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C193" s="0" t="n">
+        <v>25.672</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="194">
       <c r="A194" s="0" t="n">
         <v>193</v>
       </c>
+      <c r="B194" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C194" s="0" t="n">
+        <v>24.796</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="195">
       <c r="A195" s="0" t="n">
         <v>194</v>
       </c>
+      <c r="B195" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C195" s="0" t="n">
+        <v>24.342</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="196">
       <c r="A196" s="0" t="n">
         <v>195</v>
       </c>
+      <c r="B196" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C196" s="0" t="n">
+        <v>23.803</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="197">
       <c r="A197" s="0" t="n">
         <v>196</v>
       </c>
+      <c r="B197" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C197" s="0" t="n">
+        <v>24.309</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="198">
       <c r="A198" s="0" t="n">
         <v>197</v>
       </c>
+      <c r="B198" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C198" s="0" t="n">
+        <v>24.699</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="199">
       <c r="A199" s="0" t="n">
         <v>198</v>
       </c>
+      <c r="B199" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C199" s="0" t="n">
+        <v>24.671</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="200">
       <c r="A200" s="0" t="n">
         <v>199</v>
       </c>
+      <c r="B200" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C200" s="0" t="n">
+        <v>23.463</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="201">
       <c r="A201" s="0" t="n">
         <v>200</v>
+      </c>
+      <c r="B201" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C201" s="0" t="n">
+        <v>23.264</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="202">

</xml_diff>

<commit_message>
adding more fullerene data
</commit_message>
<xml_diff>
--- a/sknano/data/fullerenes/Cn_fullerenes.xlsx
+++ b/sknano/data/fullerenes/Cn_fullerenes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="14" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="799" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="15" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="864" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="C20" sheetId="1" state="visible" r:id="rId2"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="25">
   <si>
     <t>#</t>
   </si>
@@ -1286,7 +1286,7 @@
   </sheetPr>
   <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A64" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="C91" activeCellId="0" pane="topLeft" sqref="C91"/>
     </sheetView>
   </sheetViews>
@@ -2303,7 +2303,7 @@
   </sheetPr>
   <dimension ref="A1:C117"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A70" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A103" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="C118" activeCellId="0" pane="topLeft" sqref="C118"/>
     </sheetView>
   </sheetViews>
@@ -3617,7 +3617,7 @@
   </sheetPr>
   <dimension ref="A1:C200"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A178" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="B201" activeCellId="0" pane="topLeft" sqref="B201"/>
     </sheetView>
   </sheetViews>
@@ -5844,8 +5844,8 @@
   </sheetPr>
   <dimension ref="A1:C272"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A154" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B202" activeCellId="0" pane="topLeft" sqref="B202"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A228" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B273" activeCellId="0" pane="topLeft" sqref="B273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8064,359 +8064,785 @@
         <v>23.264</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="202">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="202">
       <c r="A202" s="0" t="n">
         <v>201</v>
+      </c>
+      <c r="B202" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C202" s="0" t="n">
+        <v>24.002</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="203">
       <c r="A203" s="0" t="n">
         <v>202</v>
       </c>
+      <c r="B203" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C203" s="0" t="n">
+        <v>23.547</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="204">
       <c r="A204" s="0" t="n">
         <v>203</v>
       </c>
+      <c r="B204" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C204" s="0" t="n">
+        <v>24.374</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="205">
       <c r="A205" s="0" t="n">
         <v>204</v>
       </c>
+      <c r="B205" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C205" s="0" t="n">
+        <v>24.286</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="206">
       <c r="A206" s="0" t="n">
         <v>205</v>
       </c>
+      <c r="B206" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C206" s="0" t="n">
+        <v>24.644</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="207">
       <c r="A207" s="0" t="n">
         <v>206</v>
       </c>
+      <c r="B207" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C207" s="0" t="n">
+        <v>24.233</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="208">
       <c r="A208" s="0" t="n">
         <v>207</v>
       </c>
+      <c r="B208" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C208" s="0" t="n">
+        <v>23.675</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="209">
       <c r="A209" s="0" t="n">
         <v>208</v>
       </c>
+      <c r="B209" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C209" s="0" t="n">
+        <v>23.425</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="210">
       <c r="A210" s="0" t="n">
         <v>209</v>
       </c>
+      <c r="B210" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C210" s="0" t="n">
+        <v>24.728</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="211">
       <c r="A211" s="0" t="n">
         <v>210</v>
       </c>
+      <c r="B211" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C211" s="0" t="n">
+        <v>25.41</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="212">
       <c r="A212" s="0" t="n">
         <v>211</v>
       </c>
+      <c r="B212" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C212" s="0" t="n">
+        <v>26.607</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="213">
       <c r="A213" s="0" t="n">
         <v>212</v>
       </c>
+      <c r="B213" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C213" s="0" t="n">
+        <v>25.452</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="214">
       <c r="A214" s="0" t="n">
         <v>213</v>
       </c>
+      <c r="B214" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C214" s="0" t="n">
+        <v>24.788</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="215">
       <c r="A215" s="0" t="n">
         <v>214</v>
       </c>
+      <c r="B215" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C215" s="0" t="n">
+        <v>23.666</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="216">
       <c r="A216" s="0" t="n">
         <v>215</v>
       </c>
+      <c r="B216" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C216" s="0" t="n">
+        <v>24.772</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="217">
       <c r="A217" s="0" t="n">
         <v>216</v>
       </c>
+      <c r="B217" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C217" s="0" t="n">
+        <v>24.2</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="218">
       <c r="A218" s="0" t="n">
         <v>217</v>
       </c>
+      <c r="B218" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C218" s="0" t="n">
+        <v>23.371</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="219">
       <c r="A219" s="0" t="n">
         <v>218</v>
       </c>
+      <c r="B219" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C219" s="0" t="n">
+        <v>23.481</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="220">
       <c r="A220" s="0" t="n">
         <v>219</v>
       </c>
+      <c r="B220" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C220" s="0" t="n">
+        <v>23.388</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="221">
       <c r="A221" s="0" t="n">
         <v>220</v>
       </c>
+      <c r="B221" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C221" s="0" t="n">
+        <v>23.848</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="222">
       <c r="A222" s="0" t="n">
         <v>221</v>
       </c>
+      <c r="B222" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C222" s="0" t="n">
+        <v>23.301</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="223">
       <c r="A223" s="0" t="n">
         <v>222</v>
       </c>
+      <c r="B223" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C223" s="0" t="n">
+        <v>23.466</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="224">
       <c r="A224" s="0" t="n">
         <v>223</v>
       </c>
+      <c r="B224" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C224" s="0" t="n">
+        <v>23.768</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="225">
       <c r="A225" s="0" t="n">
         <v>224</v>
       </c>
+      <c r="B225" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C225" s="0" t="n">
+        <v>23.867</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="226">
       <c r="A226" s="0" t="n">
         <v>225</v>
       </c>
+      <c r="B226" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C226" s="0" t="n">
+        <v>23.669</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="227">
       <c r="A227" s="0" t="n">
         <v>226</v>
       </c>
+      <c r="B227" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C227" s="0" t="n">
+        <v>23.949</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="228">
       <c r="A228" s="0" t="n">
         <v>227</v>
       </c>
+      <c r="B228" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C228" s="0" t="n">
+        <v>24.901</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="229">
       <c r="A229" s="0" t="n">
         <v>228</v>
       </c>
+      <c r="B229" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C229" s="0" t="n">
+        <v>25.077</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="230">
       <c r="A230" s="0" t="n">
         <v>229</v>
       </c>
+      <c r="B230" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C230" s="0" t="n">
+        <v>24.621</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="231">
       <c r="A231" s="0" t="n">
         <v>230</v>
       </c>
+      <c r="B231" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C231" s="0" t="n">
+        <v>24.891</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="232">
       <c r="A232" s="0" t="n">
         <v>231</v>
       </c>
+      <c r="B232" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C232" s="0" t="n">
+        <v>23.942</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="233">
       <c r="A233" s="0" t="n">
         <v>232</v>
       </c>
+      <c r="B233" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C233" s="0" t="n">
+        <v>25.008</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="234">
       <c r="A234" s="0" t="n">
         <v>233</v>
       </c>
+      <c r="B234" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C234" s="0" t="n">
+        <v>23.933</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="235">
       <c r="A235" s="0" t="n">
         <v>234</v>
       </c>
+      <c r="B235" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C235" s="0" t="n">
+        <v>24.726</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="236">
       <c r="A236" s="0" t="n">
         <v>235</v>
       </c>
+      <c r="B236" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C236" s="0" t="n">
+        <v>26.453</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="237">
       <c r="A237" s="0" t="n">
         <v>236</v>
       </c>
+      <c r="B237" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C237" s="0" t="n">
+        <v>24.301</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="238">
       <c r="A238" s="0" t="n">
         <v>237</v>
       </c>
+      <c r="B238" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C238" s="0" t="n">
+        <v>23.53</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="239">
       <c r="A239" s="0" t="n">
         <v>238</v>
       </c>
+      <c r="B239" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C239" s="0" t="n">
+        <v>24.873</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="240">
       <c r="A240" s="0" t="n">
         <v>239</v>
       </c>
+      <c r="B240" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C240" s="0" t="n">
+        <v>23.919</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="241">
       <c r="A241" s="0" t="n">
         <v>240</v>
       </c>
+      <c r="B241" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C241" s="0" t="n">
+        <v>23.065</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="242">
       <c r="A242" s="0" t="n">
         <v>241</v>
       </c>
+      <c r="B242" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C242" s="0" t="n">
+        <v>23.253</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="243">
       <c r="A243" s="0" t="n">
         <v>242</v>
       </c>
+      <c r="B243" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C243" s="0" t="n">
+        <v>24.602</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="244">
       <c r="A244" s="0" t="n">
         <v>243</v>
       </c>
+      <c r="B244" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C244" s="0" t="n">
+        <v>24.534</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="245">
       <c r="A245" s="0" t="n">
         <v>244</v>
       </c>
+      <c r="B245" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C245" s="0" t="n">
+        <v>24.178</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="246">
       <c r="A246" s="0" t="n">
         <v>245</v>
       </c>
+      <c r="B246" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C246" s="0" t="n">
+        <v>23.995</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="247">
       <c r="A247" s="0" t="n">
         <v>246</v>
       </c>
+      <c r="B247" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C247" s="0" t="n">
+        <v>23.016</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="248">
       <c r="A248" s="0" t="n">
         <v>247</v>
       </c>
+      <c r="B248" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C248" s="0" t="n">
+        <v>23.538</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="249">
       <c r="A249" s="0" t="n">
         <v>248</v>
       </c>
+      <c r="B249" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C249" s="0" t="n">
+        <v>23.063</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="250">
       <c r="A250" s="0" t="n">
         <v>249</v>
       </c>
+      <c r="B250" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C250" s="0" t="n">
+        <v>23.055</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="251">
       <c r="A251" s="0" t="n">
         <v>250</v>
       </c>
+      <c r="B251" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C251" s="0" t="n">
+        <v>23.214</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="252">
       <c r="A252" s="0" t="n">
         <v>251</v>
       </c>
+      <c r="B252" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C252" s="0" t="n">
+        <v>23.168</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="253">
       <c r="A253" s="0" t="n">
         <v>252</v>
       </c>
+      <c r="B253" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C253" s="0" t="n">
+        <v>23.545</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="254">
       <c r="A254" s="0" t="n">
         <v>253</v>
       </c>
+      <c r="B254" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C254" s="0" t="n">
+        <v>24.111</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="255">
       <c r="A255" s="0" t="n">
         <v>254</v>
       </c>
+      <c r="B255" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C255" s="0" t="n">
+        <v>23.747</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="256">
       <c r="A256" s="0" t="n">
         <v>255</v>
       </c>
+      <c r="B256" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C256" s="0" t="n">
+        <v>23.546</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="257">
       <c r="A257" s="0" t="n">
         <v>256</v>
       </c>
+      <c r="B257" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C257" s="0" t="n">
+        <v>23.861</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="258">
       <c r="A258" s="0" t="n">
         <v>257</v>
       </c>
+      <c r="B258" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C258" s="0" t="n">
+        <v>23.703</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="259">
       <c r="A259" s="0" t="n">
         <v>258</v>
       </c>
+      <c r="B259" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C259" s="0" t="n">
+        <v>24.572</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="260">
       <c r="A260" s="0" t="n">
         <v>259</v>
       </c>
+      <c r="B260" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C260" s="0" t="n">
+        <v>23.565</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="261">
       <c r="A261" s="0" t="n">
         <v>260</v>
       </c>
+      <c r="B261" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C261" s="0" t="n">
+        <v>22.811</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="262">
       <c r="A262" s="0" t="n">
         <v>261</v>
       </c>
+      <c r="B262" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C262" s="0" t="n">
+        <v>23.284</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="263">
       <c r="A263" s="0" t="n">
         <v>262</v>
       </c>
+      <c r="B263" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C263" s="0" t="n">
+        <v>22.935</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="264">
       <c r="A264" s="0" t="n">
         <v>263</v>
       </c>
+      <c r="B264" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C264" s="0" t="n">
+        <v>22.651</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="265">
       <c r="A265" s="0" t="n">
         <v>264</v>
       </c>
+      <c r="B265" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C265" s="0" t="n">
+        <v>22.83</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="266">
       <c r="A266" s="0" t="n">
         <v>265</v>
       </c>
+      <c r="B266" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C266" s="0" t="n">
+        <v>22.57</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="267">
       <c r="A267" s="0" t="n">
         <v>266</v>
       </c>
+      <c r="B267" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C267" s="0" t="n">
+        <v>22.291</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="268">
       <c r="A268" s="0" t="n">
         <v>267</v>
       </c>
+      <c r="B268" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C268" s="0" t="n">
+        <v>22.745</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="269">
       <c r="A269" s="0" t="n">
         <v>268</v>
       </c>
+      <c r="B269" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C269" s="0" t="n">
+        <v>22.699</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="270">
       <c r="A270" s="0" t="n">
         <v>269</v>
       </c>
+      <c r="B270" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C270" s="0" t="n">
+        <v>23.654</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="271">
       <c r="A271" s="0" t="n">
         <v>270</v>
       </c>
+      <c r="B271" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C271" s="0" t="n">
+        <v>22.018</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="272">
       <c r="A272" s="0" t="n">
         <v>271</v>
+      </c>
+      <c r="B272" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C272" s="0" t="n">
+        <v>22.284</v>
       </c>
     </row>
   </sheetData>
@@ -8437,8 +8863,8 @@
   </sheetPr>
   <dimension ref="A1:C438"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B50" activeCellId="0" pane="topLeft" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8461,240 +8887,528 @@
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="B2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>32.862</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="3">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="B3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>35.99</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="4">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="B4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>30.452</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="5">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="B5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>30.393</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="6">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="B6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>30.646</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="7">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="B7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>29.299</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="8">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="B8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>29.177</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="9">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
+      <c r="B9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>28.759</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="10">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
+      <c r="B10" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>30.445</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="11">
       <c r="A11" s="0" t="n">
         <v>10</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>29.177</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="12">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
+      <c r="B12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>28.855</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="13">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
+      <c r="B13" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>29.21</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="14">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
+      <c r="B14" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>30.49</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="15">
       <c r="A15" s="0" t="n">
         <v>14</v>
       </c>
+      <c r="B15" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>30.907</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="16">
       <c r="A16" s="0" t="n">
         <v>15</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>31.612</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="17">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="B17" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>29.602</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="18">
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
+      <c r="B18" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>31.948</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="19">
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
+      <c r="B19" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>29.269</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="20">
       <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
+      <c r="B20" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>28.916</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="21">
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="B21" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>29.528</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="22">
       <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
+      <c r="B22" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>29.903</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="23">
       <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
+      <c r="B23" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>28.553</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="24">
       <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
+      <c r="B24" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>27.864</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="25">
       <c r="A25" s="0" t="n">
         <v>24</v>
       </c>
+      <c r="B25" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>27.635</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="26">
       <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
+      <c r="B26" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>28.527</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="27">
       <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
+      <c r="B27" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>28.045</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="28">
       <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
+      <c r="B28" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>28.271</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="29">
       <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
+      <c r="B29" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>28.514</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="30">
       <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
+      <c r="B30" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>28.955</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="31">
       <c r="A31" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="B31" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>28.527</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="32">
       <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
+      <c r="B32" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>30.073</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="33">
       <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="B33" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>30.317</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="34">
       <c r="A34" s="0" t="n">
         <v>33</v>
       </c>
+      <c r="B34" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>28.577</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="35">
       <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
+      <c r="B35" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>27.383</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="36">
       <c r="A36" s="0" t="n">
         <v>35</v>
       </c>
+      <c r="B36" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>26.944</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="37">
       <c r="A37" s="0" t="n">
         <v>36</v>
       </c>
+      <c r="B37" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>29.248</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="38">
       <c r="A38" s="0" t="n">
         <v>37</v>
       </c>
+      <c r="B38" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>27.645</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="39">
       <c r="A39" s="0" t="n">
         <v>38</v>
       </c>
+      <c r="B39" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>29.592</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="40">
       <c r="A40" s="0" t="n">
         <v>39</v>
       </c>
+      <c r="B40" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>27.276</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="41">
       <c r="A41" s="0" t="n">
         <v>40</v>
       </c>
+      <c r="B41" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>26.724</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="42">
       <c r="A42" s="0" t="n">
         <v>41</v>
       </c>
+      <c r="B42" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>27.721</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="43">
       <c r="A43" s="0" t="n">
         <v>42</v>
       </c>
+      <c r="B43" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>27.676</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="44">
       <c r="A44" s="0" t="n">
         <v>43</v>
       </c>
+      <c r="B44" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>26.717</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="45">
       <c r="A45" s="0" t="n">
         <v>44</v>
       </c>
+      <c r="B45" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>27.455</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="46">
       <c r="A46" s="0" t="n">
         <v>45</v>
       </c>
+      <c r="B46" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>30.622</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="47">
       <c r="A47" s="0" t="n">
         <v>46</v>
       </c>
+      <c r="B47" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>27.524</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="48">
       <c r="A48" s="0" t="n">
         <v>47</v>
       </c>
+      <c r="B48" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>28.032</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="49">
       <c r="A49" s="0" t="n">
         <v>48</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>27.408</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="50">

</xml_diff>